<commit_message>
Add scatter plot data
</commit_message>
<xml_diff>
--- a/plots-drafts/toy-data/data_score_exp.xlsx
+++ b/plots-drafts/toy-data/data_score_exp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/monikafurdyna/Documents/dev/loose_analysis/Executive summary vis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/monikafurdyna/Documents/dev/pacta.executive.summary/plots-drafts/toy-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD4C78C-F6A2-E144-84D2-464D35CE3864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB71E6F-7E20-F04E-8FDD-A5060CB469D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33520" yWindow="4160" windowWidth="28040" windowHeight="17440" xr2:uid="{A60FAC01-BD50-274F-BCA2-1AA1E13B358C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="26">
   <si>
     <t>year</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>all</t>
+  </si>
+  <si>
+    <t>msci_world</t>
+  </si>
+  <si>
+    <t>benchmark</t>
   </si>
 </sst>
 </file>
@@ -464,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD66559C-116D-3942-9BE8-77D8196556AE}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -772,7 +778,7 @@
         <v>5.6347691096261254E-3</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:F27" si="0">1-E13</f>
+        <f t="shared" ref="F13:F28" si="0">1-E13</f>
         <v>0.99436523089037387</v>
       </c>
       <c r="G13">
@@ -1113,6 +1119,54 @@
       </c>
       <c r="G27">
         <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28">
+        <v>2022</v>
+      </c>
+      <c r="E28">
+        <v>0.5</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="G28">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29">
+        <v>2027</v>
+      </c>
+      <c r="E29">
+        <v>0.6</v>
+      </c>
+      <c r="F29">
+        <f t="shared" ref="F29" si="1">1-E29</f>
+        <v>0.4</v>
+      </c>
+      <c r="G29">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>